<commit_message>
feat: added function to convert matched_not_by_pmid to excel automatically, updated referenceSummary files
</commit_message>
<xml_diff>
--- a/Pubmed/Lassa/Reference_Summary_Jan29.xlsx
+++ b/Pubmed/Lassa/Reference_Summary_Jan29.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindazhou/Dropbox/___SystematicReviewsAI/LASV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E6BCBE-8294-8A40-8704-1E890F8CB170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA24BDD-82EA-E54C-B131-6B80F5BCE4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="760" windowWidth="34560" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3000" yWindow="1840" windowWidth="34560" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3977,9 +3977,6 @@
     <t>OM735989, OM735988, OM735987, OM735986, OM735985, OM735984, OM735983, OM735982, OM735981, OM735980, OM735979, OM735978, OM735977, OM735976, OM735973, OM735972, OM735971, OM735970, OM735969, OM735968, OM791219, OM791220, OM791221, OM791222, OM791227, OM791228, OM791229, OM791230, OM791231, OM791232</t>
   </si>
   <si>
-    <t>Sequences for rJosiah (HQ688673.1, HQ688675.1) and rNJ2015 (MG 812650, MG812651) have been deposited in Genbank</t>
-  </si>
-  <si>
     <t>OM735991, OM735975, KT992426-KT992431, OM791225, OM791226, OM735990, OM735974, KT992416-KT992421</t>
   </si>
   <si>
@@ -4175,6 +4172,9 @@
   <si>
     <t>LASV sequences from 2018 are deposited in GenBank, under BioProject PRJNA482058 (Data S1); sequences from 2012 to 2017 are deposited under BioProjects PRJNA482054 and PRJNA482058: MK117826 - MK118039
 MK107982 - MK107842</t>
+  </si>
+  <si>
+    <t>Sequences for rJosiah (HQ688673.1, HQ688675.1) and rNJ2015 (MG812650, MG812651) have been deposited in Genbank</t>
   </si>
 </sst>
 </file>
@@ -4308,7 +4308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4338,9 +4338,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4647,8 +4644,8 @@
   <dimension ref="A1:AD113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5252,7 +5249,7 @@
         <v>229</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L9" t="s">
         <v>225</v>
@@ -5472,7 +5469,7 @@
         <v>210</v>
       </c>
       <c r="K12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="L12" t="s">
         <v>212</v>
@@ -6814,7 +6811,7 @@
         <v>210</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L30" t="s">
         <v>225</v>
@@ -7250,7 +7247,7 @@
         <v>210</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="L36" t="s">
         <v>225</v>
@@ -11085,8 +11082,8 @@
       <c r="J86" t="s">
         <v>469</v>
       </c>
-      <c r="K86" s="12" t="s">
-        <v>600</v>
+      <c r="K86" s="2" t="s">
+        <v>604</v>
       </c>
       <c r="L86" t="s">
         <v>225</v>

</xml_diff>